<commit_message>
added serial interrupt and reading keys in the template project Arduino UNO.
</commit_message>
<xml_diff>
--- a/Boards/ArduinoUno/Template/documentation/Especificação Técnica.xlsx
+++ b/Boards/ArduinoUno/Template/documentation/Especificação Técnica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="-36" windowWidth="11460" windowHeight="9336" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="-36" windowWidth="11460" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos_Firmware" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="148">
   <si>
     <t>Microcontrolador:</t>
   </si>
@@ -455,14 +455,47 @@
     <t>5V</t>
   </si>
   <si>
-    <t>ATMEGA328P (Arduino Uno)</t>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>BTN_UP</t>
+  </si>
+  <si>
+    <t>BTN_DOWN</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>Store Program Memory Ready</t>
+  </si>
+  <si>
+    <t>Maior prioridade</t>
+  </si>
+  <si>
+    <t>Menor prioridade</t>
+  </si>
+  <si>
+    <t>SERIAL0_RX</t>
+  </si>
+  <si>
+    <t>SERIAL0_TX</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>ATMEGA328P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,8 +569,20 @@
       <color rgb="FF000000"/>
       <name val="ArialMT"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +610,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -736,24 +805,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -777,6 +828,62 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,6 +892,114 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="160020" y="1310640"/>
+          <a:ext cx="7581900" cy="4975860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Gravador:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR"/>
+            <a:t>O programa ARV_DUDE consegue gravar o arquivo .hex gerado</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" baseline="0"/>
+            <a:t> pelo compilador atmega studio 6.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR"/>
+            <a:t>O arquivo .hex e gravado usando o bootloader do proprio arduino.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR"/>
+            <a:t>Link: http://blog.zakkemble.co.uk/avrdudess-a-gui-for-avrdude/?avrdudess</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1074,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1086,20 +1301,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
@@ -1329,6 +1544,7 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1336,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1351,6 +1567,7 @@
     <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
@@ -1358,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1438,27 +1655,37 @@
       <c r="G9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="14"/>
+      <c r="K9" s="42" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="19">
+      <c r="A10" s="44">
         <v>2</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="C10" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="44"/>
       <c r="G10" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14">
+        <v>2</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="16" t="s">
         <v>59</v>
@@ -1466,19 +1693,25 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="19">
+      <c r="A11" s="44">
         <v>3</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="C11" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="44"/>
       <c r="G11" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="14">
+        <v>3</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="16" t="s">
         <v>61</v>
@@ -1486,19 +1719,25 @@
       <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="19">
+      <c r="A12" s="37">
         <v>4</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="36"/>
       <c r="G12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="14">
+        <v>4</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="16" t="s">
         <v>63</v>
@@ -1506,19 +1745,25 @@
       <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="19">
+      <c r="A13" s="37">
         <v>5</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="C13" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="36"/>
       <c r="G13" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="14">
+        <v>5</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="16" t="s">
         <v>65</v>
@@ -1526,23 +1771,25 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="33">
+      <c r="A14" s="27">
         <v>6</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="33"/>
+      <c r="E14" s="27"/>
       <c r="G14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="14">
+        <v>6</v>
+      </c>
       <c r="I14" s="14"/>
       <c r="J14" s="16" t="s">
         <v>67</v>
@@ -1550,23 +1797,25 @@
       <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="35">
+      <c r="A15" s="29">
         <v>11</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="35" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="29" t="s">
         <v>135</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <v>7</v>
+      </c>
       <c r="I15" s="14"/>
       <c r="J15" s="16" t="s">
         <v>69</v>
@@ -1574,23 +1823,25 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="38">
+      <c r="A16" s="32">
         <v>8</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="40" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="34">
         <v>0</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="14">
+        <v>8</v>
+      </c>
       <c r="I16" s="14"/>
       <c r="J16" s="16" t="s">
         <v>72</v>
@@ -1610,7 +1861,9 @@
       <c r="G17" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="14">
+        <v>9</v>
+      </c>
       <c r="I17" s="14"/>
       <c r="J17" s="16" t="s">
         <v>76</v>
@@ -1630,7 +1883,9 @@
       <c r="G18" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="14">
+        <v>10</v>
+      </c>
       <c r="I18" s="14"/>
       <c r="J18" s="16" t="s">
         <v>75</v>
@@ -1638,23 +1893,25 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="33">
+      <c r="A19" s="27">
         <v>11</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="33"/>
+      <c r="E19" s="27"/>
       <c r="G19" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="14">
+        <v>11</v>
+      </c>
       <c r="I19" s="14"/>
       <c r="J19" s="16" t="s">
         <v>50</v>
@@ -1662,23 +1919,25 @@
       <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="33">
+      <c r="A20" s="27">
         <v>12</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="33"/>
+      <c r="E20" s="27"/>
       <c r="G20" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="14">
+        <v>12</v>
+      </c>
       <c r="I20" s="14"/>
       <c r="J20" s="16" t="s">
         <v>51</v>
@@ -1686,23 +1945,25 @@
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="33">
+      <c r="A21" s="27">
         <v>13</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="33"/>
+      <c r="E21" s="27"/>
       <c r="G21" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="14"/>
+      <c r="H21" s="14">
+        <v>13</v>
+      </c>
       <c r="I21" s="14"/>
       <c r="J21" s="16" t="s">
         <v>52</v>
@@ -1710,23 +1971,25 @@
       <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="33">
+      <c r="A22" s="27">
         <v>14</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="33"/>
+      <c r="E22" s="27"/>
       <c r="G22" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="14">
+        <v>14</v>
+      </c>
       <c r="I22" s="14"/>
       <c r="J22" s="16" t="s">
         <v>53</v>
@@ -1734,23 +1997,25 @@
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="33">
+      <c r="A23" s="27">
         <v>15</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="33"/>
+      <c r="E23" s="27"/>
       <c r="G23" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="14">
+        <v>15</v>
+      </c>
       <c r="I23" s="14"/>
       <c r="J23" s="16" t="s">
         <v>54</v>
@@ -1758,19 +2023,25 @@
       <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="19">
+      <c r="A24" s="49">
         <v>16</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="48"/>
       <c r="G24" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H24" s="14"/>
+      <c r="H24" s="14">
+        <v>16</v>
+      </c>
       <c r="I24" s="14"/>
       <c r="J24" s="16" t="s">
         <v>55</v>
@@ -1778,19 +2049,25 @@
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="19">
+      <c r="A25" s="49">
         <v>17</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="48"/>
       <c r="G25" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H25" s="14"/>
+      <c r="H25" s="14">
+        <v>17</v>
+      </c>
       <c r="I25" s="14"/>
       <c r="J25" s="16" t="s">
         <v>56</v>
@@ -1810,7 +2087,9 @@
       <c r="G26" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="14"/>
+      <c r="H26" s="14">
+        <v>18</v>
+      </c>
       <c r="I26" s="14"/>
       <c r="J26" s="16" t="s">
         <v>85</v>
@@ -1827,12 +2106,16 @@
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="16" t="s">
+      <c r="H27" s="40">
+        <v>19</v>
+      </c>
+      <c r="I27" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="J27" s="41" t="s">
         <v>87</v>
       </c>
       <c r="K27" s="14"/>
@@ -1850,7 +2133,9 @@
       <c r="G28" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="14"/>
+      <c r="H28" s="14">
+        <v>20</v>
+      </c>
       <c r="I28" s="14"/>
       <c r="J28" s="16" t="s">
         <v>89</v>
@@ -1870,7 +2155,9 @@
       <c r="G29" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H29" s="14"/>
+      <c r="H29" s="14">
+        <v>21</v>
+      </c>
       <c r="I29" s="14"/>
       <c r="J29" s="16" t="s">
         <v>90</v>
@@ -1890,7 +2177,9 @@
       <c r="G30" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H30" s="14"/>
+      <c r="H30" s="14">
+        <v>22</v>
+      </c>
       <c r="I30" s="14"/>
       <c r="J30" s="16" t="s">
         <v>93</v>
@@ -1910,7 +2199,9 @@
       <c r="G31" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="H31" s="14"/>
+      <c r="H31" s="14">
+        <v>23</v>
+      </c>
       <c r="I31" s="14"/>
       <c r="J31" s="16" t="s">
         <v>94</v>
@@ -1930,7 +2221,9 @@
       <c r="G32" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H32" s="14"/>
+      <c r="H32" s="14">
+        <v>24</v>
+      </c>
       <c r="I32" s="14"/>
       <c r="J32" s="16" t="s">
         <v>97</v>
@@ -1950,9 +2243,13 @@
       <c r="G33" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H33" s="14"/>
+      <c r="H33" s="14">
+        <v>25</v>
+      </c>
       <c r="I33" s="14"/>
-      <c r="J33" s="16"/>
+      <c r="J33" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11">
@@ -1968,12 +2265,16 @@
       <c r="G34" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="H34" s="15"/>
+      <c r="H34" s="14">
+        <v>26</v>
+      </c>
       <c r="I34" s="15"/>
       <c r="J34" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="K34" s="15"/>
+        <v>140</v>
+      </c>
+      <c r="K34" s="43" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="19">

</xml_diff>